<commit_message>
Added evaluation.tex file to show the graphs. Need to add more text.
</commit_message>
<xml_diff>
--- a/Project1/report/data.xlsx
+++ b/Project1/report/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CPU" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="35">
   <si>
     <t>Threads</t>
   </si>
@@ -235,7 +235,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -475,8 +474,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="289284064"/>
-        <c:axId val="222206040"/>
+        <c:axId val="218960032"/>
+        <c:axId val="218961208"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -594,7 +593,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="289284064"/>
+        <c:axId val="218960032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -626,7 +625,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -692,7 +690,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222206040"/>
+        <c:crossAx val="218961208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -700,7 +698,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222206040"/>
+        <c:axId val="218961208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,7 +749,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -812,7 +809,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289284064"/>
+        <c:crossAx val="218960032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -826,7 +823,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -928,7 +924,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Memory Throughput</a:t>
+              <a:t>GPU Memory</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -973,7 +969,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Random Byte</c:v>
+            <c:v>Read</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -999,23 +995,37 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>GPU!$D$7:$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2^0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2^10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2^20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Mem!$D$2:$D$5</c:f>
+              <c:f>GPU!$C$7:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>25.885677999999999</c:v>
+                  <c:v>0.11509</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9941659999999999</c:v>
+                  <c:v>0.11498800000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.013649</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.0434320000000001</c:v>
+                  <c:v>2884.8678540000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1026,7 +1036,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Random Kilobyte</c:v>
+            <c:v>Write</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1052,235 +1062,37 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>GPU!$D$7:$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2^0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2^10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2^20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Mem!$D$6:$D$9</c:f>
+              <c:f>GPU!$C$10:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2119.832308</c:v>
+                  <c:v>0.115928</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1643.063629</c:v>
+                  <c:v>0.115926</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1398.413648</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1209.5116740000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Random Megabyte</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Mem!$D$10:$D$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2933.214935</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4413.2889990000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4900.0685880000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4979.2006540000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Sequenctial Byte</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Mem!$D$14:$D$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>171.45012500000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>341.06993599999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>512.41758600000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>677.63302799999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:v>Sequenctial Kilobyte</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Mem!$D$18:$D$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>4129.5745379999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6442.5726949999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7405.6789870000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2757.044281</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:v>Squenctial MegaByte</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Mem!$D$22:$D$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>3025.0214169999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4539.4095219999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5189.3382069999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1970.926903</c:v>
+                  <c:v>3656.7171109999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1297,11 +1109,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="222206432"/>
-        <c:axId val="222203688"/>
+        <c:axId val="317970000"/>
+        <c:axId val="318203808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="222206432"/>
+        <c:axId val="317970000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1328,8 +1140,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Threads</a:t>
+                  <a:t>Data</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Copy Size (Bytes)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1363,6 +1180,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1399,7 +1217,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222203688"/>
+        <c:crossAx val="318203808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1407,7 +1225,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222203688"/>
+        <c:axId val="318203808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1448,7 +1266,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Throughput (MB/sec)</a:t>
+                  <a:t>Throughput(MB/sec)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1514,7 +1332,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222206432"/>
+        <c:crossAx val="317970000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1630,12 +1448,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Memory Latency</a:t>
+              <a:t>Memory Throughput</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1703,21 +1520,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Mem!$E$2:$E$5</c:f>
+              <c:f>Mem!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.6999999999999998E-2</c:v>
+                  <c:v>25.885677999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.191</c:v>
+                  <c:v>4.9941659999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47399999999999998</c:v>
+                  <c:v>2.013649</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.46700000000000003</c:v>
+                  <c:v>2.0434320000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1756,21 +1573,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Mem!$E$6:$E$9</c:f>
+              <c:f>Mem!$D$6:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.46099999999999997</c:v>
+                  <c:v>2119.832308</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.59399999999999997</c:v>
+                  <c:v>1643.063629</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.69800000000000006</c:v>
+                  <c:v>1398.413648</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.80699999999999994</c:v>
+                  <c:v>1209.5116740000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1809,21 +1626,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Mem!$E$10:$E$13</c:f>
+              <c:f>Mem!$D$10:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>340.923</c:v>
+                  <c:v>2933.214935</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>226.58800000000002</c:v>
+                  <c:v>4413.2889990000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>204.07900000000001</c:v>
+                  <c:v>4900.0685880000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>200.83500000000001</c:v>
+                  <c:v>4979.2006540000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1862,21 +1679,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Mem!$E$14:$E$17</c:f>
+              <c:f>Mem!$D$14:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6.0000000000000001E-3</c:v>
+                  <c:v>171.45012500000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>341.06993599999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2E-3</c:v>
+                  <c:v>512.41758600000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1E-3</c:v>
+                  <c:v>677.63302799999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1915,21 +1732,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Mem!$E$18:$E$21</c:f>
+              <c:f>Mem!$D$18:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.23599999999999999</c:v>
+                  <c:v>4129.5745379999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.152</c:v>
+                  <c:v>6442.5726949999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.13200000000000001</c:v>
+                  <c:v>7405.6789870000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35399999999999998</c:v>
+                  <c:v>2757.044281</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1968,21 +1785,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Mem!$E$22:$E$25</c:f>
+              <c:f>Mem!$D$22:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>330.57599999999996</c:v>
+                  <c:v>3025.0214169999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>220.29299999999998</c:v>
+                  <c:v>4539.4095219999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>192.703</c:v>
+                  <c:v>5189.3382069999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>507.375</c:v>
+                  <c:v>1970.926903</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1999,11 +1816,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="222204080"/>
-        <c:axId val="222204472"/>
+        <c:axId val="273351304"/>
+        <c:axId val="273350912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="222204080"/>
+        <c:axId val="273351304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2035,7 +1852,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2101,7 +1917,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222204472"/>
+        <c:crossAx val="273350912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2109,7 +1925,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222204472"/>
+        <c:axId val="273350912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2150,12 +1966,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Latency (ms)</a:t>
+                  <a:t>Throughput (MB/sec)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2216,7 +2031,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222204080"/>
+        <c:crossAx val="273351304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2230,7 +2045,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2332,17 +2146,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Disk</a:t>
+              <a:t>Memory Latency</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Throughput</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2382,7 +2190,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Sequencial Write</c:v>
+            <c:v>Random Byte</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2408,43 +2216,23 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Disk!$B$3:$B$6</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2^0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2^10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2^20</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2^30</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Disk!$D$3:$D$6</c:f>
+              <c:f>Mem!$E$2:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.2462850000000001</c:v>
+                  <c:v>3.6999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>751.339608</c:v>
+                  <c:v>0.191</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1912.538708</c:v>
+                  <c:v>0.47399999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1202.808982</c:v>
+                  <c:v>0.46700000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2455,7 +2243,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Sequencial Read</c:v>
+            <c:v>Random Kilobyte</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2483,21 +2271,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Disk!$F$3:$F$6</c:f>
+              <c:f>Mem!$E$6:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.052883</c:v>
+                  <c:v>0.46099999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1846.6687830000001</c:v>
+                  <c:v>0.59399999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4132.6149690000002</c:v>
+                  <c:v>0.69800000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2634.9850879999999</c:v>
+                  <c:v>0.80699999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2508,7 +2296,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Random Write</c:v>
+            <c:v>Random Megabyte</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2536,21 +2324,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Disk!$H$3:$H$6</c:f>
+              <c:f>Mem!$E$10:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.87640700000000005</c:v>
+                  <c:v>340.923</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.770005999999999</c:v>
+                  <c:v>226.58800000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2152.4271560000002</c:v>
+                  <c:v>204.07900000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1200.269826</c:v>
+                  <c:v>200.83500000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2561,7 +2349,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Rand Read</c:v>
+            <c:v>Sequenctial Byte</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2589,21 +2377,127 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Disk!$J$3:$J$6</c:f>
+              <c:f>Mem!$E$14:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.6084369999999999</c:v>
+                  <c:v>6.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>777.06719299999997</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>169.39512999999999</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2612.2282380000001</c:v>
+                  <c:v>1E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Sequenctial Kilobyte</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Mem!$E$18:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.23599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35399999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Squenctial MegaByte</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Mem!$E$22:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>330.57599999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>220.29299999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>192.703</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>507.375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2620,11 +2514,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="289566536"/>
-        <c:axId val="289563792"/>
+        <c:axId val="273352480"/>
+        <c:axId val="273345424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="289566536"/>
+        <c:axId val="273352480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2651,12 +2545,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Read/Write Size (Bytes)</a:t>
+                  <a:t>Threads</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2686,7 +2579,6 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2723,7 +2615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289563792"/>
+        <c:crossAx val="273345424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2731,7 +2623,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="289563792"/>
+        <c:axId val="273345424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2772,12 +2664,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Throughput(MB/sec)</a:t>
+                  <a:t>Latency (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2838,7 +2729,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289566536"/>
+        <c:crossAx val="273352480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2852,7 +2743,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2958,13 +2848,12 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Latency</a:t>
+              <a:t> Throughput</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3052,21 +2941,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Disk!$E$3:$E$6</c:f>
+              <c:f>Disk!$D$3:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7.6499999999999995E-4</c:v>
+                  <c:v>1.2462850000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9999999999999995E-7</c:v>
+                  <c:v>751.339608</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1912.538708</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.9999999999999995E-7</c:v>
+                  <c:v>1202.808982</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3105,21 +2994,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Disk!$G$3:$G$6</c:f>
+              <c:f>Disk!$F$3:$F$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.1199999999999999E-4</c:v>
+                  <c:v>3.052883</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9999999999999995E-7</c:v>
+                  <c:v>1846.6687830000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4132.6149690000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2634.9850879999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3158,21 +3047,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Disk!$I$3:$I$6</c:f>
+              <c:f>Disk!$H$3:$H$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.088E-3</c:v>
+                  <c:v>0.87640700000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.6E-5</c:v>
+                  <c:v>20.770005999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2152.4271560000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.9999999999999995E-7</c:v>
+                  <c:v>1200.269826</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3211,21 +3100,21 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Disk!$K$3:$K$6</c:f>
+              <c:f>Disk!$J$3:$J$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.9299999999999999E-4</c:v>
+                  <c:v>1.6084369999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9999999999999995E-7</c:v>
+                  <c:v>777.06719299999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0000000000000002E-6</c:v>
+                  <c:v>169.39512999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2612.2282380000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3242,11 +3131,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="289559088"/>
-        <c:axId val="289564576"/>
+        <c:axId val="273346600"/>
+        <c:axId val="273348952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="289559088"/>
+        <c:axId val="273346600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3278,7 +3167,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3345,7 +3233,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289564576"/>
+        <c:crossAx val="273348952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3353,7 +3241,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="289564576"/>
+        <c:axId val="273348952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3394,12 +3282,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Latency(Sec))</a:t>
+                  <a:t>Throughput(MB/sec)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3460,7 +3347,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289559088"/>
+        <c:crossAx val="273346600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3474,7 +3361,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3542,6 +3428,624 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Disk</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Latency</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sequencial Write</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Disk!$B$3:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2^0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2^10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2^20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2^30</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Disk!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.6499999999999995E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Sequencial Read</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Disk!$G$3:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.1199999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Random Write</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Disk!$I$3:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.088E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Rand Read</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Disk!$K$3:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5.9299999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9999999999999995E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0000000000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="273347776"/>
+        <c:axId val="273348168"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="273347776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Read/Write Size (Bytes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="273348168"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="273348168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Latency(Sec))</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="273347776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3750,11 +4254,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="289564968"/>
-        <c:axId val="289565752"/>
+        <c:axId val="273349736"/>
+        <c:axId val="273350128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="289564968"/>
+        <c:axId val="273349736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3858,7 +4362,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289565752"/>
+        <c:crossAx val="273350128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3866,7 +4370,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="289565752"/>
+        <c:axId val="273350128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3973,7 +4477,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289564968"/>
+        <c:crossAx val="273349736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4054,7 +4558,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4263,11 +4767,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="289559480"/>
-        <c:axId val="289559872"/>
+        <c:axId val="273980208"/>
+        <c:axId val="273982168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="289559480"/>
+        <c:axId val="273980208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4371,7 +4875,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289559872"/>
+        <c:crossAx val="273982168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4379,7 +4883,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="289559872"/>
+        <c:axId val="273982168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4486,7 +4990,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289559480"/>
+        <c:crossAx val="273980208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4847,6 +5351,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -7866,6 +8410,509 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8404,6 +9451,41 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>504824</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>60959</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8470,7 +9552,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8537,7 +9619,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -9070,10 +10152,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C12"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9081,7 +10163,7 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -9089,7 +10171,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -9097,7 +10179,7 @@
         <v>1192.3209409999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -9105,7 +10187,7 @@
         <v>1351.923008</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -9116,7 +10198,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -9126,8 +10208,11 @@
       <c r="C7">
         <v>0.11509</v>
       </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -9137,8 +10222,11 @@
       <c r="C8">
         <v>0.11498800000000001</v>
       </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -9148,8 +10236,11 @@
       <c r="C9">
         <v>2884.8678540000001</v>
       </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -9160,7 +10251,7 @@
         <v>0.115928</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -9171,7 +10262,7 @@
         <v>0.115926</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -9184,6 +10275,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9935,7 +11027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Y36" sqref="Y36"/>
     </sheetView>
   </sheetViews>

</xml_diff>